<commit_message>
Update progbook imp interaction formatting
</commit_message>
<xml_diff>
--- a/tests/databooks/progbook_cervicalcancer.xlsx
+++ b/tests/databooks/progbook_cervicalcancer.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="38">
   <si>
     <t>Targeted to (populations)</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>Additive</t>
-  </si>
-  <si>
-    <t>Best</t>
   </si>
   <si>
     <t>Screening sensitivity</t>
@@ -1921,9 +1918,7 @@
       <c r="C2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="G2" s="6">
         <v>0.0003107232</v>
@@ -1935,7 +1930,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>31</v>
@@ -1981,9 +1976,7 @@
       <c r="C5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="6">
@@ -1997,7 +1990,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>31</v>
@@ -2043,9 +2036,7 @@
       <c r="C8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -2057,7 +2048,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>31</v>
@@ -2103,9 +2094,7 @@
       <c r="C11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -2116,11 +2105,43 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="expression" dxfId="1" priority="47">
+      <formula>COUNTIF(F11:K11,"&lt;&gt;" &amp; "")&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="48">
+      <formula>AND(COUNTIF(F11:K11,"&lt;&gt;" &amp; "")&lt;2,NOT(ISBLANK(D11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="expression" dxfId="1" priority="11">
+      <formula>COUNTIF(F2:K2,"&lt;&gt;" &amp; "")&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="12">
+      <formula>AND(COUNTIF(F2:K2,"&lt;&gt;" &amp; "")&lt;2,NOT(ISBLANK(D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="expression" dxfId="1" priority="23">
+      <formula>COUNTIF(F5:K5,"&lt;&gt;" &amp; "")&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="24">
+      <formula>AND(COUNTIF(F5:K5,"&lt;&gt;" &amp; "")&lt;2,NOT(ISBLANK(D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="expression" dxfId="1" priority="35">
+      <formula>COUNTIF(F8:K8,"&lt;&gt;" &amp; "")&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="36">
+      <formula>AND(COUNTIF(F8:K8,"&lt;&gt;" &amp; "")&lt;2,NOT(ISBLANK(D8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="expression" dxfId="2" priority="31">
+    <cfRule type="expression" dxfId="2" priority="37">
       <formula>AND('Program targeting'!$C$3&lt;&gt;"Y",NOT(ISBLANK(G11)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="32">
+    <cfRule type="expression" dxfId="3" priority="38">
       <formula>'Program targeting'!$C$3&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2133,26 +2154,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="2" priority="11">
+    <cfRule type="expression" dxfId="2" priority="13">
       <formula>AND('Program targeting'!$C$3&lt;&gt;"Y",NOT(ISBLANK(G5)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="12">
+    <cfRule type="expression" dxfId="3" priority="14">
       <formula>'Program targeting'!$C$3&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="expression" dxfId="2" priority="21">
+    <cfRule type="expression" dxfId="2" priority="25">
       <formula>AND('Program targeting'!$C$3&lt;&gt;"Y",NOT(ISBLANK(G8)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="22">
+    <cfRule type="expression" dxfId="3" priority="26">
       <formula>'Program targeting'!$C$3&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="expression" dxfId="2" priority="33">
+    <cfRule type="expression" dxfId="2" priority="39">
       <formula>AND('Program targeting'!$C$4&lt;&gt;"Y",NOT(ISBLANK(H11)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="34">
+    <cfRule type="expression" dxfId="3" priority="40">
       <formula>'Program targeting'!$C$4&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2165,26 +2186,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="2" priority="13">
+    <cfRule type="expression" dxfId="2" priority="15">
       <formula>AND('Program targeting'!$C$4&lt;&gt;"Y",NOT(ISBLANK(H5)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="14">
+    <cfRule type="expression" dxfId="3" priority="16">
       <formula>'Program targeting'!$C$4&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="2" priority="23">
+    <cfRule type="expression" dxfId="2" priority="27">
       <formula>AND('Program targeting'!$C$4&lt;&gt;"Y",NOT(ISBLANK(H8)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="24">
+    <cfRule type="expression" dxfId="3" priority="28">
       <formula>'Program targeting'!$C$4&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="2" priority="35">
+    <cfRule type="expression" dxfId="2" priority="41">
       <formula>AND('Program targeting'!$C$5&lt;&gt;"Y",NOT(ISBLANK(I11)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="36">
+    <cfRule type="expression" dxfId="3" priority="42">
       <formula>'Program targeting'!$C$5&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2197,26 +2218,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="2" priority="15">
+    <cfRule type="expression" dxfId="2" priority="17">
       <formula>AND('Program targeting'!$C$5&lt;&gt;"Y",NOT(ISBLANK(I5)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="16">
+    <cfRule type="expression" dxfId="3" priority="18">
       <formula>'Program targeting'!$C$5&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="2" priority="25">
+    <cfRule type="expression" dxfId="2" priority="29">
       <formula>AND('Program targeting'!$C$5&lt;&gt;"Y",NOT(ISBLANK(I8)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="26">
+    <cfRule type="expression" dxfId="3" priority="30">
       <formula>'Program targeting'!$C$5&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="expression" dxfId="2" priority="37">
+    <cfRule type="expression" dxfId="2" priority="43">
       <formula>AND('Program targeting'!$C$6&lt;&gt;"Y",NOT(ISBLANK(J11)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="38">
+    <cfRule type="expression" dxfId="3" priority="44">
       <formula>'Program targeting'!$C$6&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2229,26 +2250,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="expression" dxfId="2" priority="17">
+    <cfRule type="expression" dxfId="2" priority="19">
       <formula>AND('Program targeting'!$C$6&lt;&gt;"Y",NOT(ISBLANK(J5)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="18">
+    <cfRule type="expression" dxfId="3" priority="20">
       <formula>'Program targeting'!$C$6&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="expression" dxfId="2" priority="27">
+    <cfRule type="expression" dxfId="2" priority="31">
       <formula>AND('Program targeting'!$C$6&lt;&gt;"Y",NOT(ISBLANK(J8)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="28">
+    <cfRule type="expression" dxfId="3" priority="32">
       <formula>'Program targeting'!$C$6&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="expression" dxfId="2" priority="39">
+    <cfRule type="expression" dxfId="2" priority="45">
       <formula>AND('Program targeting'!$C$7&lt;&gt;"Y",NOT(ISBLANK(K11)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="40">
+    <cfRule type="expression" dxfId="3" priority="46">
       <formula>'Program targeting'!$C$7&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2261,18 +2282,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="2" priority="19">
+    <cfRule type="expression" dxfId="2" priority="21">
       <formula>AND('Program targeting'!$C$7&lt;&gt;"Y",NOT(ISBLANK(K5)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="20">
+    <cfRule type="expression" dxfId="3" priority="22">
       <formula>'Program targeting'!$C$7&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="expression" dxfId="2" priority="29">
+    <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND('Program targeting'!$C$7&lt;&gt;"Y",NOT(ISBLANK(K8)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="30">
+    <cfRule type="expression" dxfId="3" priority="34">
       <formula>'Program targeting'!$C$7&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update progbooks with 'one-off' addition
</commit_message>
<xml_diff>
--- a/tests/databooks/progbook_cervicalcancer.xlsx
+++ b/tests/databooks/progbook_cervicalcancer.xlsx
@@ -1816,31 +1816,31 @@
   </conditionalFormatting>
   <dataValidations count="10">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"$/person,$/person/year"</formula1>
+      <formula1>"$/person (one-off),$/person/year"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
       <formula1>"people/year,people"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
-      <formula1>"$/person,$/person/year"</formula1>
+      <formula1>"$/person (one-off),$/person/year"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
       <formula1>"people/year,people"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
-      <formula1>"$/person,$/person/year"</formula1>
+      <formula1>"$/person (one-off),$/person/year"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18">
       <formula1>"people/year,people"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
-      <formula1>"$/person,$/person/year"</formula1>
+      <formula1>"$/person (one-off),$/person/year"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
       <formula1>"people/year,people"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31">
-      <formula1>"$/person,$/person/year"</formula1>
+      <formula1>"$/person (one-off),$/person/year"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32">
       <formula1>"people/year,people"</formula1>

</xml_diff>